<commit_message>
Complete list of required physical interface vplans
Signed-off-by: Mike Thompson <mike@openhwgroup.org>
</commit_message>
<xml_diff>
--- a/verif/CV32E40P/VerificationPlan/VplanStatusReviews.xlsx
+++ b/verif/CV32E40P/VerificationPlan/VplanStatusReviews.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
   <si>
     <t xml:space="preserve">URL of Verification Plans:</t>
   </si>
@@ -137,6 +137,15 @@
   </si>
   <si>
     <t xml:space="preserve">physical_interfaces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sleep Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuration and Control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APU</t>
   </si>
   <si>
     <t xml:space="preserve">OBI</t>
@@ -285,7 +294,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -328,6 +337,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -407,13 +420,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:F26"/>
+  <dimension ref="B2:F29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.17"/>
@@ -624,67 +637,67 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>15</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="8" t="s">
+    <row r="20" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="8"/>
+      <c r="C20" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="D20" s="6" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="E20" s="6"/>
-      <c r="F20" s="5" t="s">
-        <v>43</v>
-      </c>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="8"/>
-      <c r="C21" s="6" t="s">
-        <v>44</v>
+      <c r="C21" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E21" s="6"/>
-      <c r="F21" s="5"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="8"/>
       <c r="C22" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B23" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="5"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="8"/>
-      <c r="C23" s="6" t="s">
+      <c r="E23" s="6"/>
+      <c r="F23" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="8"/>
@@ -692,7 +705,7 @@
         <v>47</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="5"/>
@@ -703,7 +716,7 @@
         <v>48</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="5"/>
@@ -714,18 +727,52 @@
         <v>49</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="5"/>
     </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="8"/>
+      <c r="C27" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="8"/>
+      <c r="C28" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="8"/>
+      <c r="C29" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="F29" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="B6:B11"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B20:B26"/>
-    <mergeCell ref="F20:F26"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:B29"/>
+    <mergeCell ref="F23:F29"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="https://github.com/openhwgroup/core-v-docs/tree/master/verif/CV32E40P/VerificationPlan"/>

</xml_diff>